<commit_message>
Sesipon 5 - Últimos ajustes
</commit_message>
<xml_diff>
--- a/datasets/ventas.xlsx
+++ b/datasets/ventas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\datascience-basic-cenace-2024\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D4EA794-0634-4376-BFCB-2D44BFADACDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663B8D85-52FE-44C9-BAEE-9040251D9FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37680" yWindow="4005" windowWidth="29040" windowHeight="15720" xr2:uid="{88E1AF5F-2A1C-4638-A9E4-623D0B10E0AC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="17">
   <si>
     <t>Producto</t>
   </si>
@@ -72,6 +72,21 @@
   </si>
   <si>
     <t>Venta</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Peor</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Producto Bueno</t>
+  </si>
+  <si>
+    <t>Producto Malo</t>
   </si>
 </sst>
 </file>
@@ -503,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4EB6EE6-8C85-4841-8B56-3958831777A3}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -515,9 +530,12 @@
     <col min="5" max="5" width="21.36328125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="11" max="11" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.08984375" customWidth="1"/>
+    <col min="14" max="14" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -533,8 +551,11 @@
       <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -550,8 +571,11 @@
       <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -567,8 +591,11 @@
       <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -584,8 +611,11 @@
       <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -601,8 +631,11 @@
       <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -618,8 +651,23 @@
       <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -635,8 +683,25 @@
       <c r="E7" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>COUNTIF($B$2:$B$17,H7)</f>
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f>COUNTIF($A$2:$A$17,K7)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>2</v>
       </c>
@@ -652,8 +717,25 @@
       <c r="E8" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="I8:I11" si="0">COUNTIF($B$2:$B$17,H8)</f>
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="L8:L11" si="1">COUNTIF($A$2:$A$17,K8)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>2</v>
       </c>
@@ -669,8 +751,25 @@
       <c r="E9" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>2</v>
       </c>
@@ -686,8 +785,25 @@
       <c r="E10" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>3</v>
       </c>
@@ -703,8 +819,25 @@
       <c r="E11" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>3</v>
       </c>
@@ -720,8 +853,11 @@
       <c r="E12" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>3</v>
       </c>
@@ -737,8 +873,17 @@
       <c r="E13" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
         <v>4</v>
       </c>
@@ -754,8 +899,18 @@
       <c r="E14" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f>SUMIF(B2:B17,H14,F2:F17)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>5</v>
       </c>
@@ -771,8 +926,18 @@
       <c r="E15" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I18" si="2">SUMIF(B3:B18,H15,F3:F18)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>5</v>
       </c>
@@ -788,8 +953,18 @@
       <c r="E16" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>5</v>
       </c>
@@ -805,8 +980,243 @@
       <c r="E17" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" t="s">
+        <v>15</v>
+      </c>
+      <c r="N22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>98</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23">
+        <v>23</v>
+      </c>
+      <c r="M23">
+        <f>K23*L23</f>
+        <v>69</v>
+      </c>
+      <c r="N23">
+        <v>21</v>
+      </c>
+      <c r="O23">
+        <f>K23*N23</f>
+        <v>63</v>
+      </c>
+      <c r="P23">
+        <f>M23-O23</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>279</v>
+      </c>
+      <c r="K24">
+        <v>6</v>
+      </c>
+      <c r="L24">
+        <v>28</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:N27" si="3">K24*L24</f>
+        <v>168</v>
+      </c>
+      <c r="N24">
+        <v>21</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ref="O24:O27" si="4">K24*N24</f>
+        <v>126</v>
+      </c>
+      <c r="P24">
+        <f t="shared" ref="P24:P27" si="5">M24-O24</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>175</v>
+      </c>
+      <c r="K25">
+        <v>3</v>
+      </c>
+      <c r="L25">
+        <v>25</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="N25">
+        <v>21</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>19</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>23</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="N26">
+        <v>23</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>54</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="L27">
+        <v>28</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+      <c r="N27">
+        <v>21</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P29">
+        <f>SUM(P23:P27)</f>
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="P23:P27 P29">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>